<commit_message>
redo left-right flips. switch to issueIDs
</commit_message>
<xml_diff>
--- a/dev/Issues_01.xlsx
+++ b/dev/Issues_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith Yoder\repos\SocialValuesTask\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DAE1F1-593F-43FB-899A-F7069FF3F425}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525C8270-5445-4AD3-B34B-62169027FBE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="615" windowWidth="23235" windowHeight="14250" xr2:uid="{C19661DF-E636-41D1-850F-C723F112731C}"/>
+    <workbookView xWindow="29640" yWindow="1470" windowWidth="13965" windowHeight="13995" xr2:uid="{C19661DF-E636-41D1-850F-C723F112731C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="174">
   <si>
     <t>Mask</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t>Photo_1039_02.png</t>
+  </si>
+  <si>
+    <t>IssueID</t>
   </si>
 </sst>
 </file>
@@ -946,648 +949,780 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75A9C2-F948-4BA5-944A-A99ECB2770D2}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A2" sqref="A2:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>111</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>112</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>113</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>114</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>115</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>116</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>117</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>118</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>119</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>120</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>121</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>122</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>123</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>124</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>125</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>126</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>127</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>128</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>129</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>130</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>131</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>132</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>133</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>134</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>135</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>136</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>137</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>138</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>139</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>140</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>141</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>142</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>143</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C29 C31:C44 D1:D43">
+  <conditionalFormatting sqref="D2:D29 D31:D44 E1:E43">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="D30">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="E44">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
issues with proper grammar
</commit_message>
<xml_diff>
--- a/dev/Issues_01.xlsx
+++ b/dev/Issues_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith Yoder\repos\SocialValuesTask\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A669FD7B-5E9A-404B-B9CC-93EB9F1DC8D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB097DF-BFFE-4603-A8AB-AE30DC3E3442}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="1470" windowWidth="13965" windowHeight="13995" xr2:uid="{C19661DF-E636-41D1-850F-C723F112731C}"/>
+    <workbookView xWindow="660" yWindow="1425" windowWidth="20955" windowHeight="13995" xr2:uid="{C19661DF-E636-41D1-850F-C723F112731C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="216">
   <si>
     <t>Mask</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Confederate</t>
   </si>
   <si>
-    <t>Remove public confederate memorials</t>
-  </si>
-  <si>
     <t>BLM</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>AltRight</t>
   </si>
   <si>
-    <t>Allow alt-right speakers on campuses</t>
-  </si>
-  <si>
     <t>MandatoryConsent</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>EthnicHalloween</t>
   </si>
   <si>
-    <t>Ban on ethnic halloween costumes</t>
-  </si>
-  <si>
     <t>MandatoryVaccine</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>ParksBudget</t>
   </si>
   <si>
-    <t>Cuts to national parks budget</t>
-  </si>
-  <si>
     <t>TriggerWarnings</t>
   </si>
   <si>
@@ -138,9 +126,6 @@
     <t>WarDrugs</t>
   </si>
   <si>
-    <t>War on drugs</t>
-  </si>
-  <si>
     <t>CampusCarry</t>
   </si>
   <si>
@@ -150,9 +135,6 @@
     <t>DisarmCampus</t>
   </si>
   <si>
-    <t>Gun free campus police</t>
-  </si>
-  <si>
     <t>AbolishPrison</t>
   </si>
   <si>
@@ -276,9 +258,6 @@
     <t>Lift COVID lockdowns</t>
   </si>
   <si>
-    <t>Remove Christopher Columbus statue</t>
-  </si>
-  <si>
     <t>Drones</t>
   </si>
   <si>
@@ -547,6 +526,153 @@
   </si>
   <si>
     <t>Photo_1011_02.png</t>
+  </si>
+  <si>
+    <t>IssueText</t>
+  </si>
+  <si>
+    <t>removing Confederate memorials</t>
+  </si>
+  <si>
+    <t>Remove public Confederate memorials</t>
+  </si>
+  <si>
+    <t>allowing alt-right speakers on campus</t>
+  </si>
+  <si>
+    <t>Allow alt-right speakers on campus</t>
+  </si>
+  <si>
+    <t>mandatory training on sexual consent</t>
+  </si>
+  <si>
+    <t>mandatory vaccinations</t>
+  </si>
+  <si>
+    <t>religious exemptions for discrimination laws</t>
+  </si>
+  <si>
+    <t>abortion rights</t>
+  </si>
+  <si>
+    <t>climate change legislation</t>
+  </si>
+  <si>
+    <t>affirmative action</t>
+  </si>
+  <si>
+    <t>dorms determined by gender identity</t>
+  </si>
+  <si>
+    <t>mandatory trigger warnings</t>
+  </si>
+  <si>
+    <t>tuition increases</t>
+  </si>
+  <si>
+    <t>abolishing private prisons</t>
+  </si>
+  <si>
+    <t>student worker unionization</t>
+  </si>
+  <si>
+    <t>abolishing fraternities</t>
+  </si>
+  <si>
+    <t>bathrooms restricted based on biological sex</t>
+  </si>
+  <si>
+    <t>mandatory drug tests for welfare recipients</t>
+  </si>
+  <si>
+    <t>safe injection locations</t>
+  </si>
+  <si>
+    <t>building the southern border wall</t>
+  </si>
+  <si>
+    <t>detaining migrant children</t>
+  </si>
+  <si>
+    <t>banning ethnic Halloween costumes</t>
+  </si>
+  <si>
+    <t>Ban on ethnic Halloween costumes</t>
+  </si>
+  <si>
+    <t>banning research with animals</t>
+  </si>
+  <si>
+    <t>cutting the National Parks budget</t>
+  </si>
+  <si>
+    <t>Cuts to National Parks budget</t>
+  </si>
+  <si>
+    <t>the War of Drugs</t>
+  </si>
+  <si>
+    <t>War on Drugs</t>
+  </si>
+  <si>
+    <t>on-campus concealed carry</t>
+  </si>
+  <si>
+    <t>gun-free campus police</t>
+  </si>
+  <si>
+    <t>Gun-free campus police</t>
+  </si>
+  <si>
+    <t>hardening schools/arming teachers</t>
+  </si>
+  <si>
+    <t>mask mandates</t>
+  </si>
+  <si>
+    <t>physician-assisted suicide</t>
+  </si>
+  <si>
+    <t>increased gun regulations</t>
+  </si>
+  <si>
+    <t>BDS Israel</t>
+  </si>
+  <si>
+    <t>expelling students with white nationlist views</t>
+  </si>
+  <si>
+    <t>recognizing Jerusalem as capital of Israel</t>
+  </si>
+  <si>
+    <t>legalizing of marijuana</t>
+  </si>
+  <si>
+    <t>defunding Planned Parenthood</t>
+  </si>
+  <si>
+    <t>removing police from schools</t>
+  </si>
+  <si>
+    <t>university campus being a sanctuary</t>
+  </si>
+  <si>
+    <t>defunding the police</t>
+  </si>
+  <si>
+    <t>lifting COVID lockdowns</t>
+  </si>
+  <si>
+    <t>removing Christopher Columbus statues</t>
+  </si>
+  <si>
+    <t>Remove Christopher Columbus statues</t>
+  </si>
+  <si>
+    <t>stopping police brutality</t>
+  </si>
+  <si>
+    <t>raising the minimum wage</t>
   </si>
 </sst>
 </file>
@@ -949,23 +1075,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75A9C2-F948-4BA5-944A-A99ECB2770D2}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -974,13 +1101,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -988,560 +1118,659 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>90</v>
+        <v>169</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>92</v>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>94</v>
+        <v>171</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>96</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>173</v>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>100</v>
+        <v>190</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>102</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>109</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>104</v>
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>110</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>106</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>108</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>112</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>110</v>
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>112</v>
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>114</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>115</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>116</v>
+        <v>193</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>116</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>118</v>
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>117</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>120</v>
+        <v>31</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>118</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>119</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>124</v>
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>120</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>126</v>
+        <v>198</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>121</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>128</v>
+        <v>37</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>122</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>130</v>
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>123</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>132</v>
+        <v>41</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>124</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>134</v>
+        <v>43</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>125</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>136</v>
+        <v>45</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>138</v>
+        <v>47</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>127</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>140</v>
+        <v>49</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>128</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>142</v>
+        <v>50</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>129</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>144</v>
+        <v>52</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>130</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>146</v>
+        <v>54</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>131</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>148</v>
+        <v>56</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>132</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>150</v>
+        <v>58</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>152</v>
+        <v>60</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>134</v>
       </c>
@@ -1549,180 +1778,210 @@
         <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>154</v>
+        <v>72</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>135</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>156</v>
+        <v>62</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>136</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>157</v>
+        <v>73</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>137</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>159</v>
+        <v>65</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>138</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>161</v>
+        <v>74</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>139</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>110</v>
+        <v>75</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>140</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>164</v>
+        <v>76</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>141</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>166</v>
+        <v>213</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>142</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>143</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>171</v>
+        <v>80</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29 D31:D44 E1:E43">
+  <conditionalFormatting sqref="E2:E29 E31:E44 F1:F43">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
+  <conditionalFormatting sqref="E30">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
+  <conditionalFormatting sqref="F44">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>